<commit_message>
adding TRBC Economic Sector
</commit_message>
<xml_diff>
--- a/Data/instruments_unique.xlsx
+++ b/Data/instruments_unique.xlsx
@@ -559,12 +559,12 @@
     <t>SSTE.S^J12</t>
   </si>
   <si>
+    <t>UHR.S</t>
+  </si>
+  <si>
     <t>UHRN.S</t>
   </si>
   <si>
-    <t>UHR.S</t>
-  </si>
-  <si>
     <t>SLHN.S</t>
   </si>
   <si>
@@ -2911,12 +2911,12 @@
     <t>CPRT.OQ</t>
   </si>
   <si>
+    <t>CPAY.N</t>
+  </si>
+  <si>
     <t>EVRG.OQ</t>
   </si>
   <si>
-    <t>FLT.N</t>
-  </si>
-  <si>
     <t>FTNT.OQ</t>
   </si>
   <si>
@@ -2965,12 +2965,12 @@
     <t>DOW.N</t>
   </si>
   <si>
+    <t>FOXA.OQ</t>
+  </si>
+  <si>
     <t>FOX.OQ</t>
   </si>
   <si>
-    <t>FOXA.OQ</t>
-  </si>
-  <si>
     <t>CDW.OQ</t>
   </si>
   <si>
@@ -5284,10 +5284,10 @@
     <t>PHNX.L</t>
   </si>
   <si>
+    <t>TUIJe.L^B15</t>
+  </si>
+  <si>
     <t>TUIT.L</t>
-  </si>
-  <si>
-    <t>TUIJe.L^B15</t>
   </si>
   <si>
     <t>US.MI</t>

</xml_diff>